<commit_message>
feat: count time for each test case
</commit_message>
<xml_diff>
--- a/data/Experimental Data.xlsx
+++ b/data/Experimental Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10804"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/shan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B472E-A5D0-4E4E-9F90-FAB5F2DC2393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDBFE5D-A64B-4346-8B5C-B8EC7DEC819E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19760" activeTab="1" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
   </bookViews>
   <sheets>
-    <sheet name="experiment1" sheetId="1" r:id="rId1"/>
-    <sheet name="experiment2" sheetId="4" r:id="rId2"/>
+    <sheet name="RQ1" sheetId="1" r:id="rId1"/>
+    <sheet name="RQ2" sheetId="5" r:id="rId2"/>
+    <sheet name="RQ3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -155,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +169,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF657B83"/>
+      <name val="Fira Code"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,11 +196,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,10 +867,1948 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E3B9C6-FCEA-8047-931E-C9E8F6733521}">
+  <dimension ref="A1:H101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K101" sqref="K101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.110496</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.39323999999999998</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.191742</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.18925500000000001</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.56484000000000001</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.37137300000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.26840599999999998</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.73489800000000005</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.56015599999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.34601599999999999</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.90245799999999998</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.74054900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.42630200000000001</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.0717989999999999</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.92403000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.50409199999999998</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.235204</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.1114900000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.58252800000000005</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.39994</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.297517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.66265700000000005</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.5639110000000001</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.4815389999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.74429800000000002</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.729495</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.667961</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.84034200000000003</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.8995029999999999</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.8488309999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.93705899999999998</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.0668769999999999</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.0316839999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.0355669999999999</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.231662</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.2133929999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.130285</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.3997320000000002</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2.3969</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.22834</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.5656669999999999</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2.5782370000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.3255980000000001</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2.7306879999999998</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2.7634159999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.424685</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2.9163890000000001</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2.9423010000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.5220180000000001</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3.0894379999999999</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3.1238519999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.620428</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3.2513359999999998</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3.3023039999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.715023</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3.4184329999999998</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3.4914320000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.814371</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3.5806480000000001</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3.6707489999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.910976</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.747004</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3.853021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.007533</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.9128280000000002</v>
+      </c>
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23" s="2">
+        <v>4.0297929999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2.1039270000000001</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4.0782429999999996</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4.221991</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2.2009080000000001</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4.248882</v>
+      </c>
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25" s="2">
+        <v>4.3997710000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2.294896</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.447908</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26" s="2">
+        <v>4.5880489999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2.3932340000000001</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4.6479350000000004</v>
+      </c>
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27" s="2">
+        <v>4.7649689999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2.4893830000000001</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4.8425260000000003</v>
+      </c>
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28" s="2">
+        <v>4.9526960000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2.5909450000000001</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5.0359040000000004</v>
+      </c>
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29" s="2">
+        <v>5.1426030000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2.6854330000000002</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5.2351419999999997</v>
+      </c>
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5.3317839999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2.7858770000000002</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5.4262920000000001</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31" s="2">
+        <v>5.5213580000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2.8824399999999999</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5.6273910000000003</v>
+      </c>
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32" s="2">
+        <v>5.7084650000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2.9780950000000002</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" s="2">
+        <v>5.8221189999999998</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33" s="2">
+        <v>5.9030040000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3.073855</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="E34" s="2">
+        <v>6.0155839999999996</v>
+      </c>
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34" s="2">
+        <v>6.1232800000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3.173578</v>
+      </c>
+      <c r="D35">
+        <v>34</v>
+      </c>
+      <c r="E35" s="2">
+        <v>6.2186050000000002</v>
+      </c>
+      <c r="G35">
+        <v>34</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6.3330570000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3.2696079999999998</v>
+      </c>
+      <c r="D36">
+        <v>35</v>
+      </c>
+      <c r="E36" s="2">
+        <v>6.4147509999999999</v>
+      </c>
+      <c r="G36">
+        <v>35</v>
+      </c>
+      <c r="H36" s="2">
+        <v>6.5179559999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3.366295</v>
+      </c>
+      <c r="D37">
+        <v>36</v>
+      </c>
+      <c r="E37" s="2">
+        <v>6.6094670000000004</v>
+      </c>
+      <c r="G37">
+        <v>36</v>
+      </c>
+      <c r="H37" s="2">
+        <v>6.7343909999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>3.4835759999999998</v>
+      </c>
+      <c r="D38">
+        <v>37</v>
+      </c>
+      <c r="E38" s="2">
+        <v>6.8096430000000003</v>
+      </c>
+      <c r="G38">
+        <v>37</v>
+      </c>
+      <c r="H38" s="2">
+        <v>6.9598060000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>3.5978720000000002</v>
+      </c>
+      <c r="D39">
+        <v>38</v>
+      </c>
+      <c r="E39" s="2">
+        <v>7.0053349999999996</v>
+      </c>
+      <c r="G39">
+        <v>38</v>
+      </c>
+      <c r="H39" s="2">
+        <v>7.183821</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>3.7195399999999998</v>
+      </c>
+      <c r="D40">
+        <v>39</v>
+      </c>
+      <c r="E40" s="2">
+        <v>7.2068029999999998</v>
+      </c>
+      <c r="G40">
+        <v>39</v>
+      </c>
+      <c r="H40" s="2">
+        <v>7.4027349999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3.8344049999999998</v>
+      </c>
+      <c r="D41">
+        <v>40</v>
+      </c>
+      <c r="E41" s="2">
+        <v>7.4011529999999999</v>
+      </c>
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="H41" s="2">
+        <v>7.6255420000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>3.9482400000000002</v>
+      </c>
+      <c r="D42">
+        <v>41</v>
+      </c>
+      <c r="E42" s="2">
+        <v>7.6012320000000004</v>
+      </c>
+      <c r="G42">
+        <v>41</v>
+      </c>
+      <c r="H42" s="2">
+        <v>7.8537679999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>4.0627769999999996</v>
+      </c>
+      <c r="D43">
+        <v>42</v>
+      </c>
+      <c r="E43" s="2">
+        <v>7.8027329999999999</v>
+      </c>
+      <c r="G43">
+        <v>42</v>
+      </c>
+      <c r="H43" s="2">
+        <v>8.0786490000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>4.1772679999999998</v>
+      </c>
+      <c r="D44">
+        <v>43</v>
+      </c>
+      <c r="E44" s="2">
+        <v>7.9980539999999998</v>
+      </c>
+      <c r="G44">
+        <v>43</v>
+      </c>
+      <c r="H44" s="2">
+        <v>8.3047939999999993</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>4.2914880000000002</v>
+      </c>
+      <c r="D45">
+        <v>44</v>
+      </c>
+      <c r="E45" s="2">
+        <v>8.1955749999999998</v>
+      </c>
+      <c r="G45">
+        <v>44</v>
+      </c>
+      <c r="H45" s="2">
+        <v>8.5233170000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>4.40733</v>
+      </c>
+      <c r="D46">
+        <v>45</v>
+      </c>
+      <c r="E46" s="2">
+        <v>8.3910250000000008</v>
+      </c>
+      <c r="G46">
+        <v>45</v>
+      </c>
+      <c r="H46" s="2">
+        <v>8.747681</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>4.5221119999999999</v>
+      </c>
+      <c r="D47">
+        <v>46</v>
+      </c>
+      <c r="E47" s="2">
+        <v>8.5935400000000008</v>
+      </c>
+      <c r="G47">
+        <v>46</v>
+      </c>
+      <c r="H47" s="2">
+        <v>8.9669430000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>4.6361480000000004</v>
+      </c>
+      <c r="D48">
+        <v>47</v>
+      </c>
+      <c r="E48" s="2">
+        <v>8.7988870000000006</v>
+      </c>
+      <c r="G48">
+        <v>47</v>
+      </c>
+      <c r="H48" s="2">
+        <v>9.1872120000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>4.749676</v>
+      </c>
+      <c r="D49">
+        <v>48</v>
+      </c>
+      <c r="E49" s="2">
+        <v>8.9966679999999997</v>
+      </c>
+      <c r="G49">
+        <v>48</v>
+      </c>
+      <c r="H49" s="2">
+        <v>9.4002909999999993</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2">
+        <v>4.8669390000000003</v>
+      </c>
+      <c r="D50">
+        <v>49</v>
+      </c>
+      <c r="E50" s="2">
+        <v>9.1868870000000005</v>
+      </c>
+      <c r="G50">
+        <v>49</v>
+      </c>
+      <c r="H50" s="2">
+        <v>9.6225120000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2">
+        <v>4.9818720000000001</v>
+      </c>
+      <c r="D51">
+        <v>50</v>
+      </c>
+      <c r="E51" s="2">
+        <v>9.3895250000000008</v>
+      </c>
+      <c r="G51">
+        <v>50</v>
+      </c>
+      <c r="H51" s="2">
+        <v>9.8372270000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2">
+        <v>5.0969439999999997</v>
+      </c>
+      <c r="D52">
+        <v>51</v>
+      </c>
+      <c r="E52" s="2">
+        <v>9.5845330000000004</v>
+      </c>
+      <c r="G52">
+        <v>51</v>
+      </c>
+      <c r="H52" s="2">
+        <v>10.050521</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2">
+        <v>5.2118659999999997</v>
+      </c>
+      <c r="D53">
+        <v>52</v>
+      </c>
+      <c r="E53" s="2">
+        <v>9.7945869999999999</v>
+      </c>
+      <c r="G53">
+        <v>52</v>
+      </c>
+      <c r="H53" s="2">
+        <v>10.266282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2">
+        <v>5.3265650000000004</v>
+      </c>
+      <c r="D54">
+        <v>53</v>
+      </c>
+      <c r="E54" s="2">
+        <v>9.9941300000000002</v>
+      </c>
+      <c r="G54">
+        <v>53</v>
+      </c>
+      <c r="H54" s="2">
+        <v>10.481199999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2">
+        <v>5.4430880000000004</v>
+      </c>
+      <c r="D55">
+        <v>54</v>
+      </c>
+      <c r="E55" s="2">
+        <v>10.186175</v>
+      </c>
+      <c r="G55">
+        <v>54</v>
+      </c>
+      <c r="H55" s="2">
+        <v>10.694224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2">
+        <v>5.5576949999999998</v>
+      </c>
+      <c r="D56">
+        <v>55</v>
+      </c>
+      <c r="E56" s="2">
+        <v>10.388688</v>
+      </c>
+      <c r="G56">
+        <v>55</v>
+      </c>
+      <c r="H56" s="2">
+        <v>10.909144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2">
+        <v>5.6720030000000001</v>
+      </c>
+      <c r="D57">
+        <v>56</v>
+      </c>
+      <c r="E57" s="2">
+        <v>10.586544</v>
+      </c>
+      <c r="G57">
+        <v>56</v>
+      </c>
+      <c r="H57" s="2">
+        <v>11.122941000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2">
+        <v>5.7864940000000002</v>
+      </c>
+      <c r="D58">
+        <v>57</v>
+      </c>
+      <c r="E58" s="2">
+        <v>10.794983</v>
+      </c>
+      <c r="G58">
+        <v>57</v>
+      </c>
+      <c r="H58" s="2">
+        <v>11.335976</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2">
+        <v>5.9002400000000002</v>
+      </c>
+      <c r="D59">
+        <v>58</v>
+      </c>
+      <c r="E59" s="2">
+        <v>10.986997000000001</v>
+      </c>
+      <c r="G59">
+        <v>58</v>
+      </c>
+      <c r="H59" s="2">
+        <v>11.549224000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2">
+        <v>6.0154649999999998</v>
+      </c>
+      <c r="D60">
+        <v>59</v>
+      </c>
+      <c r="E60" s="2">
+        <v>11.185466</v>
+      </c>
+      <c r="G60">
+        <v>59</v>
+      </c>
+      <c r="H60" s="2">
+        <v>11.765855</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2">
+        <v>6.1314739999999999</v>
+      </c>
+      <c r="D61">
+        <v>60</v>
+      </c>
+      <c r="E61" s="2">
+        <v>11.384554</v>
+      </c>
+      <c r="G61">
+        <v>60</v>
+      </c>
+      <c r="H61" s="2">
+        <v>11.978668000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2">
+        <v>6.2457520000000004</v>
+      </c>
+      <c r="D62">
+        <v>61</v>
+      </c>
+      <c r="E62" s="2">
+        <v>11.583722</v>
+      </c>
+      <c r="G62">
+        <v>61</v>
+      </c>
+      <c r="H62" s="2">
+        <v>12.198178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2">
+        <v>6.3603500000000004</v>
+      </c>
+      <c r="D63">
+        <v>62</v>
+      </c>
+      <c r="E63" s="2">
+        <v>11.793938000000001</v>
+      </c>
+      <c r="G63">
+        <v>62</v>
+      </c>
+      <c r="H63" s="2">
+        <v>12.411322</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2">
+        <v>6.4760980000000004</v>
+      </c>
+      <c r="D64">
+        <v>63</v>
+      </c>
+      <c r="E64" s="2">
+        <v>11.989000000000001</v>
+      </c>
+      <c r="G64">
+        <v>63</v>
+      </c>
+      <c r="H64" s="2">
+        <v>12.630770999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2">
+        <v>6.5904639999999999</v>
+      </c>
+      <c r="D65">
+        <v>64</v>
+      </c>
+      <c r="E65" s="2">
+        <v>12.183858000000001</v>
+      </c>
+      <c r="G65">
+        <v>64</v>
+      </c>
+      <c r="H65" s="2">
+        <v>12.853768000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2">
+        <v>6.7037279999999999</v>
+      </c>
+      <c r="D66">
+        <v>65</v>
+      </c>
+      <c r="E66" s="2">
+        <v>12.390224</v>
+      </c>
+      <c r="G66">
+        <v>65</v>
+      </c>
+      <c r="H66" s="2">
+        <v>13.064444999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2">
+        <v>6.8204019999999996</v>
+      </c>
+      <c r="D67">
+        <v>66</v>
+      </c>
+      <c r="E67" s="2">
+        <v>12.586824999999999</v>
+      </c>
+      <c r="G67">
+        <v>66</v>
+      </c>
+      <c r="H67" s="2">
+        <v>13.277498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2">
+        <v>6.9367140000000003</v>
+      </c>
+      <c r="D68">
+        <v>67</v>
+      </c>
+      <c r="E68" s="2">
+        <v>12.789507</v>
+      </c>
+      <c r="G68">
+        <v>67</v>
+      </c>
+      <c r="H68" s="2">
+        <v>13.490447</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
+        <v>7.0509649999999997</v>
+      </c>
+      <c r="D69">
+        <v>68</v>
+      </c>
+      <c r="E69" s="2">
+        <v>12.980487999999999</v>
+      </c>
+      <c r="G69">
+        <v>68</v>
+      </c>
+      <c r="H69" s="2">
+        <v>13.707604</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2">
+        <v>7.1678689999999996</v>
+      </c>
+      <c r="D70">
+        <v>69</v>
+      </c>
+      <c r="E70" s="2">
+        <v>13.180754</v>
+      </c>
+      <c r="G70">
+        <v>69</v>
+      </c>
+      <c r="H70" s="2">
+        <v>13.923228999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="2">
+        <v>7.2827029999999997</v>
+      </c>
+      <c r="D71">
+        <v>70</v>
+      </c>
+      <c r="E71" s="2">
+        <v>13.379735999999999</v>
+      </c>
+      <c r="G71">
+        <v>70</v>
+      </c>
+      <c r="H71" s="2">
+        <v>14.136049</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2">
+        <v>7.3983299999999996</v>
+      </c>
+      <c r="D72">
+        <v>71</v>
+      </c>
+      <c r="E72" s="2">
+        <v>13.575523</v>
+      </c>
+      <c r="G72">
+        <v>71</v>
+      </c>
+      <c r="H72" s="2">
+        <v>14.348136999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2">
+        <v>7.5139519999999997</v>
+      </c>
+      <c r="D73">
+        <v>72</v>
+      </c>
+      <c r="E73" s="2">
+        <v>13.773830999999999</v>
+      </c>
+      <c r="G73">
+        <v>72</v>
+      </c>
+      <c r="H73" s="2">
+        <v>14.566215</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2">
+        <v>7.6315489999999997</v>
+      </c>
+      <c r="D74">
+        <v>73</v>
+      </c>
+      <c r="E74" s="2">
+        <v>13.969060000000001</v>
+      </c>
+      <c r="G74">
+        <v>73</v>
+      </c>
+      <c r="H74" s="2">
+        <v>14.78018</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2">
+        <v>7.745158</v>
+      </c>
+      <c r="D75">
+        <v>74</v>
+      </c>
+      <c r="E75" s="2">
+        <v>14.165641000000001</v>
+      </c>
+      <c r="G75">
+        <v>74</v>
+      </c>
+      <c r="H75" s="2">
+        <v>14.996180000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2">
+        <v>7.8608950000000002</v>
+      </c>
+      <c r="D76">
+        <v>75</v>
+      </c>
+      <c r="E76" s="2">
+        <v>14.362501</v>
+      </c>
+      <c r="G76">
+        <v>75</v>
+      </c>
+      <c r="H76" s="2">
+        <v>15.210663</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2">
+        <v>7.9757670000000003</v>
+      </c>
+      <c r="D77">
+        <v>76</v>
+      </c>
+      <c r="E77" s="2">
+        <v>14.556716</v>
+      </c>
+      <c r="G77">
+        <v>76</v>
+      </c>
+      <c r="H77" s="2">
+        <v>15.423264</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2">
+        <v>8.0911570000000008</v>
+      </c>
+      <c r="D78">
+        <v>77</v>
+      </c>
+      <c r="E78" s="2">
+        <v>14.749832</v>
+      </c>
+      <c r="G78">
+        <v>77</v>
+      </c>
+      <c r="H78" s="2">
+        <v>15.647686999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2">
+        <v>8.2063889999999997</v>
+      </c>
+      <c r="D79">
+        <v>78</v>
+      </c>
+      <c r="E79" s="2">
+        <v>14.955057</v>
+      </c>
+      <c r="G79">
+        <v>78</v>
+      </c>
+      <c r="H79" s="2">
+        <v>15.874720999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="2">
+        <v>8.3217370000000006</v>
+      </c>
+      <c r="D80">
+        <v>79</v>
+      </c>
+      <c r="E80" s="2">
+        <v>15.156946</v>
+      </c>
+      <c r="G80">
+        <v>79</v>
+      </c>
+      <c r="H80" s="2">
+        <v>16.08558</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2">
+        <v>8.4374110000000009</v>
+      </c>
+      <c r="D81">
+        <v>80</v>
+      </c>
+      <c r="E81" s="2">
+        <v>15.351265</v>
+      </c>
+      <c r="G81">
+        <v>80</v>
+      </c>
+      <c r="H81" s="2">
+        <v>16.299289999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2">
+        <v>8.5517310000000002</v>
+      </c>
+      <c r="D82">
+        <v>81</v>
+      </c>
+      <c r="E82" s="2">
+        <v>15.548021</v>
+      </c>
+      <c r="G82">
+        <v>81</v>
+      </c>
+      <c r="H82" s="2">
+        <v>16.511725999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2">
+        <v>8.6655960000000007</v>
+      </c>
+      <c r="D83">
+        <v>82</v>
+      </c>
+      <c r="E83" s="2">
+        <v>15.753926</v>
+      </c>
+      <c r="G83">
+        <v>82</v>
+      </c>
+      <c r="H83" s="2">
+        <v>16.731935</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2">
+        <v>8.7817439999999998</v>
+      </c>
+      <c r="D84">
+        <v>83</v>
+      </c>
+      <c r="E84" s="2">
+        <v>15.948214999999999</v>
+      </c>
+      <c r="G84">
+        <v>83</v>
+      </c>
+      <c r="H84" s="2">
+        <v>16.95506</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="2">
+        <v>8.8994070000000001</v>
+      </c>
+      <c r="D85">
+        <v>84</v>
+      </c>
+      <c r="E85" s="2">
+        <v>16.153856000000001</v>
+      </c>
+      <c r="G85">
+        <v>84</v>
+      </c>
+      <c r="H85" s="2">
+        <v>17.176099000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="2">
+        <v>9.0172550000000005</v>
+      </c>
+      <c r="G86">
+        <v>85</v>
+      </c>
+      <c r="H86" s="2">
+        <v>17.387656</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="2">
+        <v>9.1325570000000003</v>
+      </c>
+      <c r="G87">
+        <v>86</v>
+      </c>
+      <c r="H87" s="2">
+        <v>17.597950999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="2">
+        <v>9.2466930000000005</v>
+      </c>
+      <c r="G88">
+        <v>87</v>
+      </c>
+      <c r="H88" s="2">
+        <v>17.817523000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="2">
+        <v>9.3627749999999992</v>
+      </c>
+      <c r="G89">
+        <v>88</v>
+      </c>
+      <c r="H89" s="2">
+        <v>18.033528</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="2">
+        <v>9.4783840000000001</v>
+      </c>
+      <c r="G90">
+        <v>89</v>
+      </c>
+      <c r="H90" s="2">
+        <v>18.247541999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="2">
+        <v>9.5935089999999992</v>
+      </c>
+      <c r="G91">
+        <v>90</v>
+      </c>
+      <c r="H91" s="2">
+        <v>18.460032999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="2">
+        <v>9.7082329999999999</v>
+      </c>
+      <c r="G92">
+        <v>91</v>
+      </c>
+      <c r="H92" s="2">
+        <v>18.673907</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="2">
+        <v>9.823283</v>
+      </c>
+      <c r="G93">
+        <v>92</v>
+      </c>
+      <c r="H93" s="2">
+        <v>18.885524</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="2">
+        <v>9.9365500000000004</v>
+      </c>
+      <c r="G94">
+        <v>93</v>
+      </c>
+      <c r="H94" s="2">
+        <v>19.099135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="2">
+        <v>10.050983</v>
+      </c>
+      <c r="G95">
+        <v>94</v>
+      </c>
+      <c r="H95" s="2">
+        <v>19.314038</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="2">
+        <v>10.165514999999999</v>
+      </c>
+      <c r="G96">
+        <v>95</v>
+      </c>
+      <c r="H96" s="2">
+        <v>19.525483999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="2">
+        <v>10.280249</v>
+      </c>
+      <c r="G97">
+        <v>96</v>
+      </c>
+      <c r="H97" s="2">
+        <v>19.741924000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="2">
+        <v>10.395536</v>
+      </c>
+      <c r="G98">
+        <v>97</v>
+      </c>
+      <c r="H98" s="2">
+        <v>19.960214000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="2">
+        <v>10.511096999999999</v>
+      </c>
+      <c r="G99">
+        <v>98</v>
+      </c>
+      <c r="H99" s="2">
+        <v>20.174828999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="2">
+        <v>10.626408</v>
+      </c>
+      <c r="G100">
+        <v>99</v>
+      </c>
+      <c r="H100" s="2">
+        <v>20.386503000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="2">
+        <v>10.739374</v>
+      </c>
+      <c r="G101">
+        <v>100</v>
+      </c>
+      <c r="H101" s="2">
+        <v>20.600042999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE35945D-E516-AB45-8B17-F8B3ECBEF8EA}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: measure time for each case
</commit_message>
<xml_diff>
--- a/data/Experimental Data.xlsx
+++ b/data/Experimental Data.xlsx
@@ -8,26 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/shan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDBFE5D-A64B-4346-8B5C-B8EC7DEC819E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3E3734-448A-BC43-AC86-023DB39EFC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19760" activeTab="1" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19760" activeTab="2" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
   </bookViews>
   <sheets>
-    <sheet name="RQ1" sheetId="1" r:id="rId1"/>
-    <sheet name="RQ2" sheetId="5" r:id="rId2"/>
-    <sheet name="RQ3" sheetId="4" r:id="rId3"/>
+    <sheet name="RQ1-Table" sheetId="1" r:id="rId1"/>
+    <sheet name="RQ1-Charts" sheetId="5" r:id="rId2"/>
+    <sheet name="RQ2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>No</t>
   </si>
@@ -92,9 +102,6 @@
     <t>Counter Example</t>
   </si>
   <si>
-    <t>OT</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
@@ -150,6 +157,36 @@
   </si>
   <si>
     <t>Memory (GB)</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Automata</t>
+  </si>
+  <si>
+    <t>Transition</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Mode-Coverage</t>
+  </si>
+  <si>
+    <t>Transition-Coverage</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>Pruned</t>
+  </si>
+  <si>
+    <t>PruningRatio</t>
   </si>
 </sst>
 </file>
@@ -176,12 +213,18 @@
       <name val="Fira Code"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -196,12 +239,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,66 +568,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FACF2A-E248-534C-8FDA-43D644C552B5}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="2" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -586,22 +658,40 @@
         <v>2</v>
       </c>
       <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3">
+        <v>117</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="I3">
+      <c r="N3">
         <v>1.52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -612,22 +702,40 @@
         <v>2</v>
       </c>
       <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="6">
+        <v>5913</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="N4">
         <v>64.989999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -638,22 +746,40 @@
         <v>3</v>
       </c>
       <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5">
+        <v>27</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.77</v>
+      </c>
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="M5" t="s">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="N5">
         <v>0.53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -664,19 +790,37 @@
         <v>3</v>
       </c>
       <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6">
+        <v>222</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.47</v>
+      </c>
+      <c r="K6" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>1.071</v>
+      </c>
+      <c r="N6">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -687,19 +831,37 @@
         <v>2</v>
       </c>
       <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7">
+        <v>84</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K7" t="s">
         <v>19</v>
       </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>4.2229999999999999</v>
+      </c>
+      <c r="N7">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -710,19 +872,37 @@
         <v>3</v>
       </c>
       <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>34</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K8" t="s">
         <v>19</v>
       </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="N8">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -733,22 +913,40 @@
         <v>2</v>
       </c>
       <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="M9" t="s">
         <v>19</v>
       </c>
-      <c r="I9">
+      <c r="N9">
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -759,22 +957,40 @@
         <v>3</v>
       </c>
       <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>47</v>
+      </c>
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.36</v>
+      </c>
+      <c r="K10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L10">
+        <v>1.56</v>
+      </c>
+      <c r="M10" t="s">
         <v>20</v>
       </c>
-      <c r="I10">
+      <c r="N10">
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -785,22 +1001,40 @@
         <v>2</v>
       </c>
       <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" s="6">
+        <v>11986</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="K11" t="s">
         <v>20</v>
       </c>
-      <c r="H11" t="s">
+      <c r="L11">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="M11" t="s">
         <v>20</v>
       </c>
-      <c r="I11">
+      <c r="N11">
         <v>8.91</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -811,19 +1045,37 @@
         <v>4</v>
       </c>
       <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12">
+        <v>627</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="K12" t="s">
         <v>19</v>
       </c>
-      <c r="I12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="N12">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -834,31 +1086,51 @@
         <v>2</v>
       </c>
       <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>28</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.64</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="K13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" t="s">
+      <c r="L13">
+        <v>0.191</v>
+      </c>
+      <c r="M13" t="s">
         <v>20</v>
       </c>
-      <c r="I13">
+      <c r="N13">
         <v>0.39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="10">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -870,43 +1142,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E3B9C6-FCEA-8047-931E-C9E8F6733521}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.110496</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>0.39323999999999998</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>0.191742</v>
       </c>
     </row>
@@ -914,19 +1188,19 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.18925500000000001</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0.56484000000000001</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0.37137300000000001</v>
       </c>
     </row>
@@ -934,19 +1208,19 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.26840599999999998</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0.73489800000000005</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0.56015599999999999</v>
       </c>
     </row>
@@ -954,19 +1228,19 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.34601599999999999</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>0.90245799999999998</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>0.74054900000000001</v>
       </c>
     </row>
@@ -974,19 +1248,19 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.42630200000000001</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>1.0717989999999999</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>0.92403000000000002</v>
       </c>
     </row>
@@ -994,19 +1268,19 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.50409199999999998</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1.235204</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>1.1114900000000001</v>
       </c>
     </row>
@@ -1014,19 +1288,19 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.58252800000000005</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>1.39994</v>
       </c>
       <c r="G8">
         <v>7</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>1.297517</v>
       </c>
     </row>
@@ -1034,19 +1308,19 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>0.66265700000000005</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1.5639110000000001</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>1.4815389999999999</v>
       </c>
     </row>
@@ -1054,19 +1328,19 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.74429800000000002</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1.729495</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>1.667961</v>
       </c>
     </row>
@@ -1074,19 +1348,19 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0.84034200000000003</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1.8995029999999999</v>
       </c>
       <c r="G11">
         <v>10</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>1.8488309999999999</v>
       </c>
     </row>
@@ -1094,19 +1368,19 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0.93705899999999998</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>2.0668769999999999</v>
       </c>
       <c r="G12">
         <v>11</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>2.0316839999999998</v>
       </c>
     </row>
@@ -1114,19 +1388,19 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>1.0355669999999999</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>2.231662</v>
       </c>
       <c r="G13">
         <v>12</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>2.2133929999999999</v>
       </c>
     </row>
@@ -1134,19 +1408,19 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>1.130285</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>2.3997320000000002</v>
       </c>
       <c r="G14">
         <v>13</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>2.3969</v>
       </c>
     </row>
@@ -1154,19 +1428,19 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>1.22834</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>2.5656669999999999</v>
       </c>
       <c r="G15">
         <v>14</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>2.5782370000000001</v>
       </c>
     </row>
@@ -1174,19 +1448,19 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1.3255980000000001</v>
       </c>
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>2.7306879999999998</v>
       </c>
       <c r="G16">
         <v>15</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>2.7634159999999999</v>
       </c>
     </row>
@@ -1194,19 +1468,19 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>1.424685</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>2.9163890000000001</v>
       </c>
       <c r="G17">
         <v>16</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>2.9423010000000001</v>
       </c>
     </row>
@@ -1214,19 +1488,19 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1.5220180000000001</v>
       </c>
       <c r="D18">
         <v>17</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>3.0894379999999999</v>
       </c>
       <c r="G18">
         <v>17</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>3.1238519999999999</v>
       </c>
     </row>
@@ -1234,19 +1508,19 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1.620428</v>
       </c>
       <c r="D19">
         <v>18</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>3.2513359999999998</v>
       </c>
       <c r="G19">
         <v>18</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
         <v>3.3023039999999999</v>
       </c>
     </row>
@@ -1254,19 +1528,19 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1.715023</v>
       </c>
       <c r="D20">
         <v>19</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>3.4184329999999998</v>
       </c>
       <c r="G20">
         <v>19</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>3.4914320000000001</v>
       </c>
     </row>
@@ -1274,19 +1548,19 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1.814371</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>3.5806480000000001</v>
       </c>
       <c r="G21">
         <v>20</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>3.6707489999999998</v>
       </c>
     </row>
@@ -1294,19 +1568,19 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1.910976</v>
       </c>
       <c r="D22">
         <v>21</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>3.747004</v>
       </c>
       <c r="G22">
         <v>21</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
         <v>3.853021</v>
       </c>
     </row>
@@ -1314,19 +1588,19 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>2.007533</v>
       </c>
       <c r="D23">
         <v>22</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>3.9128280000000002</v>
       </c>
       <c r="G23">
         <v>22</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>4.0297929999999997</v>
       </c>
     </row>
@@ -1334,19 +1608,19 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>2.1039270000000001</v>
       </c>
       <c r="D24">
         <v>23</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>4.0782429999999996</v>
       </c>
       <c r="G24">
         <v>23</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>4.221991</v>
       </c>
     </row>
@@ -1354,19 +1628,19 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>2.2009080000000001</v>
       </c>
       <c r="D25">
         <v>24</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>4.248882</v>
       </c>
       <c r="G25">
         <v>24</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>4.3997710000000003</v>
       </c>
     </row>
@@ -1374,19 +1648,19 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2.294896</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>4.447908</v>
       </c>
       <c r="G26">
         <v>25</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>4.5880489999999998</v>
       </c>
     </row>
@@ -1394,19 +1668,19 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>2.3932340000000001</v>
       </c>
       <c r="D27">
         <v>26</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>4.6479350000000004</v>
       </c>
       <c r="G27">
         <v>26</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>4.7649689999999998</v>
       </c>
     </row>
@@ -1414,19 +1688,19 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>2.4893830000000001</v>
       </c>
       <c r="D28">
         <v>27</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>4.8425260000000003</v>
       </c>
       <c r="G28">
         <v>27</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>4.9526960000000004</v>
       </c>
     </row>
@@ -1434,19 +1708,19 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>2.5909450000000001</v>
       </c>
       <c r="D29">
         <v>28</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>5.0359040000000004</v>
       </c>
       <c r="G29">
         <v>28</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>5.1426030000000003</v>
       </c>
     </row>
@@ -1454,19 +1728,19 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>2.6854330000000002</v>
       </c>
       <c r="D30">
         <v>29</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>5.2351419999999997</v>
       </c>
       <c r="G30">
         <v>29</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>5.3317839999999999</v>
       </c>
     </row>
@@ -1474,19 +1748,19 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>2.7858770000000002</v>
       </c>
       <c r="D31">
         <v>30</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>5.4262920000000001</v>
       </c>
       <c r="G31">
         <v>30</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
         <v>5.5213580000000002</v>
       </c>
     </row>
@@ -1494,19 +1768,19 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>2.8824399999999999</v>
       </c>
       <c r="D32">
         <v>31</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>5.6273910000000003</v>
       </c>
       <c r="G32">
         <v>31</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>5.7084650000000003</v>
       </c>
     </row>
@@ -1514,19 +1788,19 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>2.9780950000000002</v>
       </c>
       <c r="D33">
         <v>32</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>5.8221189999999998</v>
       </c>
       <c r="G33">
         <v>32</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
         <v>5.9030040000000001</v>
       </c>
     </row>
@@ -1534,19 +1808,19 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>3.073855</v>
       </c>
       <c r="D34">
         <v>33</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>6.0155839999999996</v>
       </c>
       <c r="G34">
         <v>33</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="1">
         <v>6.1232800000000003</v>
       </c>
     </row>
@@ -1554,19 +1828,19 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>3.173578</v>
       </c>
       <c r="D35">
         <v>34</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>6.2186050000000002</v>
       </c>
       <c r="G35">
         <v>34</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="1">
         <v>6.3330570000000002</v>
       </c>
     </row>
@@ -1574,19 +1848,19 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>3.2696079999999998</v>
       </c>
       <c r="D36">
         <v>35</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="1">
         <v>6.4147509999999999</v>
       </c>
       <c r="G36">
         <v>35</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="1">
         <v>6.5179559999999999</v>
       </c>
     </row>
@@ -1594,19 +1868,19 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>3.366295</v>
       </c>
       <c r="D37">
         <v>36</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="1">
         <v>6.6094670000000004</v>
       </c>
       <c r="G37">
         <v>36</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="1">
         <v>6.7343909999999996</v>
       </c>
     </row>
@@ -1614,19 +1888,19 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>3.4835759999999998</v>
       </c>
       <c r="D38">
         <v>37</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>6.8096430000000003</v>
       </c>
       <c r="G38">
         <v>37</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="1">
         <v>6.9598060000000004</v>
       </c>
     </row>
@@ -1634,19 +1908,19 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>3.5978720000000002</v>
       </c>
       <c r="D39">
         <v>38</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>7.0053349999999996</v>
       </c>
       <c r="G39">
         <v>38</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="1">
         <v>7.183821</v>
       </c>
     </row>
@@ -1654,19 +1928,19 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>3.7195399999999998</v>
       </c>
       <c r="D40">
         <v>39</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>7.2068029999999998</v>
       </c>
       <c r="G40">
         <v>39</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="1">
         <v>7.4027349999999998</v>
       </c>
     </row>
@@ -1674,19 +1948,19 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>3.8344049999999998</v>
       </c>
       <c r="D41">
         <v>40</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>7.4011529999999999</v>
       </c>
       <c r="G41">
         <v>40</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>7.6255420000000003</v>
       </c>
     </row>
@@ -1694,19 +1968,19 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>3.9482400000000002</v>
       </c>
       <c r="D42">
         <v>41</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>7.6012320000000004</v>
       </c>
       <c r="G42">
         <v>41</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>7.8537679999999996</v>
       </c>
     </row>
@@ -1714,19 +1988,19 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>4.0627769999999996</v>
       </c>
       <c r="D43">
         <v>42</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>7.8027329999999999</v>
       </c>
       <c r="G43">
         <v>42</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="1">
         <v>8.0786490000000004</v>
       </c>
     </row>
@@ -1734,19 +2008,19 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>4.1772679999999998</v>
       </c>
       <c r="D44">
         <v>43</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>7.9980539999999998</v>
       </c>
       <c r="G44">
         <v>43</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="1">
         <v>8.3047939999999993</v>
       </c>
     </row>
@@ -1754,19 +2028,19 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>4.2914880000000002</v>
       </c>
       <c r="D45">
         <v>44</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>8.1955749999999998</v>
       </c>
       <c r="G45">
         <v>44</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="1">
         <v>8.5233170000000005</v>
       </c>
     </row>
@@ -1774,19 +2048,19 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>4.40733</v>
       </c>
       <c r="D46">
         <v>45</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>8.3910250000000008</v>
       </c>
       <c r="G46">
         <v>45</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="1">
         <v>8.747681</v>
       </c>
     </row>
@@ -1794,19 +2068,19 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>4.5221119999999999</v>
       </c>
       <c r="D47">
         <v>46</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="1">
         <v>8.5935400000000008</v>
       </c>
       <c r="G47">
         <v>46</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="1">
         <v>8.9669430000000006</v>
       </c>
     </row>
@@ -1814,19 +2088,19 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>4.6361480000000004</v>
       </c>
       <c r="D48">
         <v>47</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="1">
         <v>8.7988870000000006</v>
       </c>
       <c r="G48">
         <v>47</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="1">
         <v>9.1872120000000006</v>
       </c>
     </row>
@@ -1834,19 +2108,19 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>4.749676</v>
       </c>
       <c r="D49">
         <v>48</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="1">
         <v>8.9966679999999997</v>
       </c>
       <c r="G49">
         <v>48</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="1">
         <v>9.4002909999999993</v>
       </c>
     </row>
@@ -1854,19 +2128,19 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>4.8669390000000003</v>
       </c>
       <c r="D50">
         <v>49</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="1">
         <v>9.1868870000000005</v>
       </c>
       <c r="G50">
         <v>49</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="1">
         <v>9.6225120000000004</v>
       </c>
     </row>
@@ -1874,19 +2148,19 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>4.9818720000000001</v>
       </c>
       <c r="D51">
         <v>50</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="1">
         <v>9.3895250000000008</v>
       </c>
       <c r="G51">
         <v>50</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="1">
         <v>9.8372270000000004</v>
       </c>
     </row>
@@ -1894,19 +2168,19 @@
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>5.0969439999999997</v>
       </c>
       <c r="D52">
         <v>51</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="1">
         <v>9.5845330000000004</v>
       </c>
       <c r="G52">
         <v>51</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="1">
         <v>10.050521</v>
       </c>
     </row>
@@ -1914,19 +2188,19 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>5.2118659999999997</v>
       </c>
       <c r="D53">
         <v>52</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="1">
         <v>9.7945869999999999</v>
       </c>
       <c r="G53">
         <v>52</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="1">
         <v>10.266282</v>
       </c>
     </row>
@@ -1934,19 +2208,19 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>5.3265650000000004</v>
       </c>
       <c r="D54">
         <v>53</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="1">
         <v>9.9941300000000002</v>
       </c>
       <c r="G54">
         <v>53</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="1">
         <v>10.481199999999999</v>
       </c>
     </row>
@@ -1954,19 +2228,19 @@
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>5.4430880000000004</v>
       </c>
       <c r="D55">
         <v>54</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="1">
         <v>10.186175</v>
       </c>
       <c r="G55">
         <v>54</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="1">
         <v>10.694224</v>
       </c>
     </row>
@@ -1974,19 +2248,19 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>5.5576949999999998</v>
       </c>
       <c r="D56">
         <v>55</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="1">
         <v>10.388688</v>
       </c>
       <c r="G56">
         <v>55</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="1">
         <v>10.909144</v>
       </c>
     </row>
@@ -1994,19 +2268,19 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>5.6720030000000001</v>
       </c>
       <c r="D57">
         <v>56</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="1">
         <v>10.586544</v>
       </c>
       <c r="G57">
         <v>56</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57" s="1">
         <v>11.122941000000001</v>
       </c>
     </row>
@@ -2014,19 +2288,19 @@
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>5.7864940000000002</v>
       </c>
       <c r="D58">
         <v>57</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="1">
         <v>10.794983</v>
       </c>
       <c r="G58">
         <v>57</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="1">
         <v>11.335976</v>
       </c>
     </row>
@@ -2034,19 +2308,19 @@
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>5.9002400000000002</v>
       </c>
       <c r="D59">
         <v>58</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="1">
         <v>10.986997000000001</v>
       </c>
       <c r="G59">
         <v>58</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59" s="1">
         <v>11.549224000000001</v>
       </c>
     </row>
@@ -2054,19 +2328,19 @@
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>6.0154649999999998</v>
       </c>
       <c r="D60">
         <v>59</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="1">
         <v>11.185466</v>
       </c>
       <c r="G60">
         <v>59</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60" s="1">
         <v>11.765855</v>
       </c>
     </row>
@@ -2074,19 +2348,19 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>6.1314739999999999</v>
       </c>
       <c r="D61">
         <v>60</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="1">
         <v>11.384554</v>
       </c>
       <c r="G61">
         <v>60</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="1">
         <v>11.978668000000001</v>
       </c>
     </row>
@@ -2094,19 +2368,19 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>6.2457520000000004</v>
       </c>
       <c r="D62">
         <v>61</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="1">
         <v>11.583722</v>
       </c>
       <c r="G62">
         <v>61</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="1">
         <v>12.198178</v>
       </c>
     </row>
@@ -2114,19 +2388,19 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>6.3603500000000004</v>
       </c>
       <c r="D63">
         <v>62</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="1">
         <v>11.793938000000001</v>
       </c>
       <c r="G63">
         <v>62</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63" s="1">
         <v>12.411322</v>
       </c>
     </row>
@@ -2134,19 +2408,19 @@
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>6.4760980000000004</v>
       </c>
       <c r="D64">
         <v>63</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="1">
         <v>11.989000000000001</v>
       </c>
       <c r="G64">
         <v>63</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64" s="1">
         <v>12.630770999999999</v>
       </c>
     </row>
@@ -2154,19 +2428,19 @@
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>6.5904639999999999</v>
       </c>
       <c r="D65">
         <v>64</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="1">
         <v>12.183858000000001</v>
       </c>
       <c r="G65">
         <v>64</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="1">
         <v>12.853768000000001</v>
       </c>
     </row>
@@ -2174,19 +2448,19 @@
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>6.7037279999999999</v>
       </c>
       <c r="D66">
         <v>65</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="1">
         <v>12.390224</v>
       </c>
       <c r="G66">
         <v>65</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="1">
         <v>13.064444999999999</v>
       </c>
     </row>
@@ -2194,19 +2468,19 @@
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>6.8204019999999996</v>
       </c>
       <c r="D67">
         <v>66</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="1">
         <v>12.586824999999999</v>
       </c>
       <c r="G67">
         <v>66</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67" s="1">
         <v>13.277498</v>
       </c>
     </row>
@@ -2214,19 +2488,19 @@
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>6.9367140000000003</v>
       </c>
       <c r="D68">
         <v>67</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="1">
         <v>12.789507</v>
       </c>
       <c r="G68">
         <v>67</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68" s="1">
         <v>13.490447</v>
       </c>
     </row>
@@ -2234,19 +2508,19 @@
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>7.0509649999999997</v>
       </c>
       <c r="D69">
         <v>68</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="1">
         <v>12.980487999999999</v>
       </c>
       <c r="G69">
         <v>68</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69" s="1">
         <v>13.707604</v>
       </c>
     </row>
@@ -2254,19 +2528,19 @@
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>7.1678689999999996</v>
       </c>
       <c r="D70">
         <v>69</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="1">
         <v>13.180754</v>
       </c>
       <c r="G70">
         <v>69</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70" s="1">
         <v>13.923228999999999</v>
       </c>
     </row>
@@ -2274,19 +2548,19 @@
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>7.2827029999999997</v>
       </c>
       <c r="D71">
         <v>70</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="1">
         <v>13.379735999999999</v>
       </c>
       <c r="G71">
         <v>70</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71" s="1">
         <v>14.136049</v>
       </c>
     </row>
@@ -2294,19 +2568,19 @@
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>7.3983299999999996</v>
       </c>
       <c r="D72">
         <v>71</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="1">
         <v>13.575523</v>
       </c>
       <c r="G72">
         <v>71</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72" s="1">
         <v>14.348136999999999</v>
       </c>
     </row>
@@ -2314,19 +2588,19 @@
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>7.5139519999999997</v>
       </c>
       <c r="D73">
         <v>72</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="1">
         <v>13.773830999999999</v>
       </c>
       <c r="G73">
         <v>72</v>
       </c>
-      <c r="H73" s="2">
+      <c r="H73" s="1">
         <v>14.566215</v>
       </c>
     </row>
@@ -2334,19 +2608,19 @@
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>7.6315489999999997</v>
       </c>
       <c r="D74">
         <v>73</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="1">
         <v>13.969060000000001</v>
       </c>
       <c r="G74">
         <v>73</v>
       </c>
-      <c r="H74" s="2">
+      <c r="H74" s="1">
         <v>14.78018</v>
       </c>
     </row>
@@ -2354,19 +2628,19 @@
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>7.745158</v>
       </c>
       <c r="D75">
         <v>74</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="1">
         <v>14.165641000000001</v>
       </c>
       <c r="G75">
         <v>74</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75" s="1">
         <v>14.996180000000001</v>
       </c>
     </row>
@@ -2374,19 +2648,19 @@
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>7.8608950000000002</v>
       </c>
       <c r="D76">
         <v>75</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="1">
         <v>14.362501</v>
       </c>
       <c r="G76">
         <v>75</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76" s="1">
         <v>15.210663</v>
       </c>
     </row>
@@ -2394,19 +2668,19 @@
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>7.9757670000000003</v>
       </c>
       <c r="D77">
         <v>76</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77" s="1">
         <v>14.556716</v>
       </c>
       <c r="G77">
         <v>76</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77" s="1">
         <v>15.423264</v>
       </c>
     </row>
@@ -2414,19 +2688,19 @@
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>8.0911570000000008</v>
       </c>
       <c r="D78">
         <v>77</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78" s="1">
         <v>14.749832</v>
       </c>
       <c r="G78">
         <v>77</v>
       </c>
-      <c r="H78" s="2">
+      <c r="H78" s="1">
         <v>15.647686999999999</v>
       </c>
     </row>
@@ -2434,19 +2708,19 @@
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>8.2063889999999997</v>
       </c>
       <c r="D79">
         <v>78</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="1">
         <v>14.955057</v>
       </c>
       <c r="G79">
         <v>78</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H79" s="1">
         <v>15.874720999999999</v>
       </c>
     </row>
@@ -2454,19 +2728,19 @@
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>8.3217370000000006</v>
       </c>
       <c r="D80">
         <v>79</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80" s="1">
         <v>15.156946</v>
       </c>
       <c r="G80">
         <v>79</v>
       </c>
-      <c r="H80" s="2">
+      <c r="H80" s="1">
         <v>16.08558</v>
       </c>
     </row>
@@ -2474,19 +2748,19 @@
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>8.4374110000000009</v>
       </c>
       <c r="D81">
         <v>80</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81" s="1">
         <v>15.351265</v>
       </c>
       <c r="G81">
         <v>80</v>
       </c>
-      <c r="H81" s="2">
+      <c r="H81" s="1">
         <v>16.299289999999999</v>
       </c>
     </row>
@@ -2494,19 +2768,19 @@
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>8.5517310000000002</v>
       </c>
       <c r="D82">
         <v>81</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="1">
         <v>15.548021</v>
       </c>
       <c r="G82">
         <v>81</v>
       </c>
-      <c r="H82" s="2">
+      <c r="H82" s="1">
         <v>16.511725999999999</v>
       </c>
     </row>
@@ -2514,19 +2788,19 @@
       <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>8.6655960000000007</v>
       </c>
       <c r="D83">
         <v>82</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="1">
         <v>15.753926</v>
       </c>
       <c r="G83">
         <v>82</v>
       </c>
-      <c r="H83" s="2">
+      <c r="H83" s="1">
         <v>16.731935</v>
       </c>
     </row>
@@ -2534,19 +2808,19 @@
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>8.7817439999999998</v>
       </c>
       <c r="D84">
         <v>83</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="1">
         <v>15.948214999999999</v>
       </c>
       <c r="G84">
         <v>83</v>
       </c>
-      <c r="H84" s="2">
+      <c r="H84" s="1">
         <v>16.95506</v>
       </c>
     </row>
@@ -2554,19 +2828,19 @@
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>8.8994070000000001</v>
       </c>
       <c r="D85">
         <v>84</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="1">
         <v>16.153856000000001</v>
       </c>
       <c r="G85">
         <v>84</v>
       </c>
-      <c r="H85" s="2">
+      <c r="H85" s="1">
         <v>17.176099000000001</v>
       </c>
     </row>
@@ -2574,13 +2848,13 @@
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>9.0172550000000005</v>
       </c>
       <c r="G86">
         <v>85</v>
       </c>
-      <c r="H86" s="2">
+      <c r="H86" s="1">
         <v>17.387656</v>
       </c>
     </row>
@@ -2588,13 +2862,13 @@
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>9.1325570000000003</v>
       </c>
       <c r="G87">
         <v>86</v>
       </c>
-      <c r="H87" s="2">
+      <c r="H87" s="1">
         <v>17.597950999999998</v>
       </c>
     </row>
@@ -2602,13 +2876,13 @@
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>9.2466930000000005</v>
       </c>
       <c r="G88">
         <v>87</v>
       </c>
-      <c r="H88" s="2">
+      <c r="H88" s="1">
         <v>17.817523000000001</v>
       </c>
     </row>
@@ -2616,13 +2890,13 @@
       <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>9.3627749999999992</v>
       </c>
       <c r="G89">
         <v>88</v>
       </c>
-      <c r="H89" s="2">
+      <c r="H89" s="1">
         <v>18.033528</v>
       </c>
     </row>
@@ -2630,13 +2904,13 @@
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>9.4783840000000001</v>
       </c>
       <c r="G90">
         <v>89</v>
       </c>
-      <c r="H90" s="2">
+      <c r="H90" s="1">
         <v>18.247541999999999</v>
       </c>
     </row>
@@ -2644,13 +2918,13 @@
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>9.5935089999999992</v>
       </c>
       <c r="G91">
         <v>90</v>
       </c>
-      <c r="H91" s="2">
+      <c r="H91" s="1">
         <v>18.460032999999999</v>
       </c>
     </row>
@@ -2658,13 +2932,13 @@
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>9.7082329999999999</v>
       </c>
       <c r="G92">
         <v>91</v>
       </c>
-      <c r="H92" s="2">
+      <c r="H92" s="1">
         <v>18.673907</v>
       </c>
     </row>
@@ -2672,13 +2946,13 @@
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>9.823283</v>
       </c>
       <c r="G93">
         <v>92</v>
       </c>
-      <c r="H93" s="2">
+      <c r="H93" s="1">
         <v>18.885524</v>
       </c>
     </row>
@@ -2686,13 +2960,13 @@
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>9.9365500000000004</v>
       </c>
       <c r="G94">
         <v>93</v>
       </c>
-      <c r="H94" s="2">
+      <c r="H94" s="1">
         <v>19.099135</v>
       </c>
     </row>
@@ -2700,13 +2974,13 @@
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>10.050983</v>
       </c>
       <c r="G95">
         <v>94</v>
       </c>
-      <c r="H95" s="2">
+      <c r="H95" s="1">
         <v>19.314038</v>
       </c>
     </row>
@@ -2714,13 +2988,13 @@
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>10.165514999999999</v>
       </c>
       <c r="G96">
         <v>95</v>
       </c>
-      <c r="H96" s="2">
+      <c r="H96" s="1">
         <v>19.525483999999999</v>
       </c>
     </row>
@@ -2728,13 +3002,13 @@
       <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="1">
         <v>10.280249</v>
       </c>
       <c r="G97">
         <v>96</v>
       </c>
-      <c r="H97" s="2">
+      <c r="H97" s="1">
         <v>19.741924000000001</v>
       </c>
     </row>
@@ -2742,13 +3016,13 @@
       <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>10.395536</v>
       </c>
       <c r="G98">
         <v>97</v>
       </c>
-      <c r="H98" s="2">
+      <c r="H98" s="1">
         <v>19.960214000000001</v>
       </c>
     </row>
@@ -2756,13 +3030,13 @@
       <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>10.511096999999999</v>
       </c>
       <c r="G99">
         <v>98</v>
       </c>
-      <c r="H99" s="2">
+      <c r="H99" s="1">
         <v>20.174828999999999</v>
       </c>
     </row>
@@ -2770,13 +3044,13 @@
       <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>10.626408</v>
       </c>
       <c r="G100">
         <v>99</v>
       </c>
-      <c r="H100" s="2">
+      <c r="H100" s="1">
         <v>20.386503000000001</v>
       </c>
     </row>
@@ -2784,13 +3058,13 @@
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="1">
         <v>10.739374</v>
       </c>
       <c r="G101">
         <v>100</v>
       </c>
-      <c r="H101" s="2">
+      <c r="H101" s="1">
         <v>20.600042999999999</v>
       </c>
     </row>
@@ -2806,50 +3080,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE35945D-E516-AB45-8B17-F8B3ECBEF8EA}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="13" max="13" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -2864,21 +3151,34 @@
         <v>1</v>
       </c>
       <c r="F2">
+        <v>58</v>
+      </c>
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>I2/H2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="H2">
+      <c r="L2">
         <v>7.63</v>
       </c>
-      <c r="I2">
+      <c r="M2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -2893,21 +3193,34 @@
         <v>2</v>
       </c>
       <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3">
+        <v>84540</v>
+      </c>
+      <c r="I3" s="6">
+        <v>84531</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J11" si="0">I3/H3</f>
+        <v>0.99989354151880772</v>
+      </c>
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>84.3</v>
       </c>
-      <c r="I3">
+      <c r="M3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -2922,21 +3235,34 @@
         <v>2</v>
       </c>
       <c r="F4">
+        <v>49</v>
+      </c>
+      <c r="G4">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4">
+        <v>1692</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1683</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0.99468085106382975</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>131</v>
       </c>
-      <c r="I4">
+      <c r="M4">
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -2951,21 +3277,34 @@
         <v>3</v>
       </c>
       <c r="F5">
+        <v>47</v>
+      </c>
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5">
+        <v>864</v>
+      </c>
+      <c r="I5">
+        <v>840</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>82.5</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <v>2.6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -2980,21 +3319,34 @@
         <v>2</v>
       </c>
       <c r="F6">
+        <v>34</v>
+      </c>
+      <c r="G6">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6">
+        <v>370</v>
+      </c>
+      <c r="I6">
+        <v>340</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.91891891891891897</v>
+      </c>
+      <c r="K6" t="s">
         <v>19</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>132</v>
       </c>
-      <c r="I6">
+      <c r="M6">
         <v>2.6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -3009,21 +3361,34 @@
         <v>2</v>
       </c>
       <c r="F7">
+        <v>47</v>
+      </c>
+      <c r="G7">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7">
+        <v>20043000</v>
+      </c>
+      <c r="I7" s="6">
+        <v>20042976</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.99999880257446494</v>
+      </c>
+      <c r="K7" t="s">
         <v>19</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>1370</v>
       </c>
-      <c r="I7">
+      <c r="M7">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -3038,21 +3403,34 @@
         <v>3</v>
       </c>
       <c r="F8">
+        <v>39</v>
+      </c>
+      <c r="G8">
         <v>11</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8">
+        <v>2096640</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2096590</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.99997615231990233</v>
+      </c>
+      <c r="K8" t="s">
         <v>19</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>508</v>
       </c>
-      <c r="I8">
+      <c r="M8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -3067,21 +3445,34 @@
         <v>2</v>
       </c>
       <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
         <v>6</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9">
+        <v>960</v>
+      </c>
+      <c r="I9">
+        <v>934</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0.97291666666666665</v>
+      </c>
+      <c r="K9" t="s">
         <v>19</v>
       </c>
-      <c r="H9">
+      <c r="L9">
         <v>75.2</v>
       </c>
-      <c r="I9">
+      <c r="M9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -3096,21 +3487,34 @@
         <v>1</v>
       </c>
       <c r="F10">
+        <v>48</v>
+      </c>
+      <c r="G10">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
         <v>19</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>20.8</v>
       </c>
-      <c r="I10">
+      <c r="M10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -3125,20 +3529,34 @@
         <v>3</v>
       </c>
       <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="G11">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11">
+        <v>93416</v>
+      </c>
+      <c r="I11" s="6">
+        <v>93393</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.99975378950072791</v>
+      </c>
+      <c r="K11" t="s">
         <v>20</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>207</v>
       </c>
-      <c r="I11">
+      <c r="M11">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>